<commit_message>
update for single stock
</commit_message>
<xml_diff>
--- a/monitor_xlsx/20260129.xlsx
+++ b/monitor_xlsx/20260129.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="總覽" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="詳細數據" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="個股籌碼" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -37,8 +38,18 @@
       <b val="1"/>
       <sz val="14"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
+    </font>
+    <font>
+      <color rgb="00008000"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -49,6 +60,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00CCCCCC"/>
         <bgColor rgb="00CCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
       </patternFill>
     </fill>
   </fills>
@@ -64,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -74,6 +91,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -545,12 +567,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5465.8$</t>
+          <t>5318.4$</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+3.10%</t>
+          <t>+0.32%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -665,12 +687,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>30.0億</t>
+          <t>34.08億</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>600.1億</t>
+          <t>681.57億</t>
         </is>
       </c>
     </row>
@@ -717,13 +739,13 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>134.57%</t>
+          <t>131.55%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>134.57%</t>
+          <t>131.55%</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -888,7 +910,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>30.0億</t>
+          <t>34.08億</t>
         </is>
       </c>
     </row>
@@ -900,7 +922,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>600.1億</t>
+          <t>681.57億</t>
         </is>
       </c>
     </row>
@@ -1002,7 +1024,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>134.57%</t>
+          <t>131.55%</t>
         </is>
       </c>
     </row>
@@ -1021,4 +1043,910 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="14" customWidth="1" min="15" max="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>個股籌碼監控報告 - 20260129</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>股票代號</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>股票名稱</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>收盤價</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>漲跌幅(%)</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>成交量(張)</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>外資當日(張)</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>外資5日累計</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>投信當日(張)</t>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>投信5日累計</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="inlineStr">
+        <is>
+          <t>自營商當日(張)</t>
+        </is>
+      </c>
+      <c r="K3" s="5" t="inlineStr">
+        <is>
+          <t>融資增減(張)</t>
+        </is>
+      </c>
+      <c r="L3" s="5" t="inlineStr">
+        <is>
+          <t>融資5日累計</t>
+        </is>
+      </c>
+      <c r="M3" s="5" t="inlineStr">
+        <is>
+          <t>借券增減(張)</t>
+        </is>
+      </c>
+      <c r="N3" s="5" t="inlineStr">
+        <is>
+          <t>MA20乖離(%)</t>
+        </is>
+      </c>
+      <c r="O3" s="5" t="inlineStr">
+        <is>
+          <t>籌碼評價</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0050</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0050</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>73.75</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>-0.61</v>
+      </c>
+      <c r="E4" t="n">
+        <v>119914</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>-28279</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3361</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1700</v>
+      </c>
+      <c r="I4" t="n">
+        <v>866</v>
+      </c>
+      <c r="J4" t="n">
+        <v>44503</v>
+      </c>
+      <c r="K4" t="n">
+        <v>7062</v>
+      </c>
+      <c r="L4" t="n">
+        <v>36064</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-3975503</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>偏多</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>00708L</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>S&amp;P黃金正2</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>210</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-541</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-60</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-70</v>
+      </c>
+      <c r="J5" t="n">
+        <v>9094</v>
+      </c>
+      <c r="K5" t="n">
+        <v>9338</v>
+      </c>
+      <c r="L5" t="n">
+        <v>38507</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-22201</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>主力積極賣出</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1519</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>華城</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4703</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>174</v>
+      </c>
+      <c r="G6" t="n">
+        <v>799</v>
+      </c>
+      <c r="H6" t="n">
+        <v>59</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-588</v>
+      </c>
+      <c r="J6" t="n">
+        <v>157</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2739</v>
+      </c>
+      <c r="L6" t="n">
+        <v>14321</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-78648</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-2.12</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>中性</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1605</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>華新</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>44</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="E7" t="n">
+        <v>286253</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>-4211</v>
+      </c>
+      <c r="G7" t="n">
+        <v>23921</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6125</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7012</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7756</v>
+      </c>
+      <c r="K7" t="n">
+        <v>84102</v>
+      </c>
+      <c r="L7" t="n">
+        <v>388683</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-1104426</v>
+      </c>
+      <c r="N7" t="n">
+        <v>9.07</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>偏多</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2308</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>台達電</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1255</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>-1.95</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13505</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>-947</v>
+      </c>
+      <c r="G8" t="n">
+        <v>370</v>
+      </c>
+      <c r="H8" t="n">
+        <v>56</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1818</v>
+      </c>
+      <c r="J8" t="n">
+        <v>475</v>
+      </c>
+      <c r="K8" t="n">
+        <v>6754</v>
+      </c>
+      <c r="L8" t="n">
+        <v>41447</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-648590</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>偏多</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2330</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>台積電</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1805</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>-0.82</v>
+      </c>
+      <c r="E9" t="n">
+        <v>36079</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>-8629</v>
+      </c>
+      <c r="G9" t="n">
+        <v>143</v>
+      </c>
+      <c r="H9" t="n">
+        <v>15</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3765</v>
+      </c>
+      <c r="J9" t="n">
+        <v>691</v>
+      </c>
+      <c r="K9" t="n">
+        <v>19907</v>
+      </c>
+      <c r="L9" t="n">
+        <v>101732</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-6482788</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>偏多</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2344</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>華邦電</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>130</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="E10" t="n">
+        <v>391188</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>-9530</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-29698</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2445</v>
+      </c>
+      <c r="I10" t="n">
+        <v>18007</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6032</v>
+      </c>
+      <c r="K10" t="n">
+        <v>147377</v>
+      </c>
+      <c r="L10" t="n">
+        <v>713069</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-1105481</v>
+      </c>
+      <c r="N10" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>偏空</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2383</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>台光電</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1790</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>-5.79</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4284</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>-334</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4787</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-440</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-343</v>
+      </c>
+      <c r="J11" t="n">
+        <v>324</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2053</v>
+      </c>
+      <c r="L11" t="n">
+        <v>10459</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-89489</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>中性</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>3661</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>世芯-KY</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3270</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>-2.97</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2536</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <v>-610</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-203</v>
+      </c>
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-143</v>
+      </c>
+      <c r="J12" t="n">
+        <v>127</v>
+      </c>
+      <c r="K12" t="n">
+        <v>5961</v>
+      </c>
+      <c r="L12" t="n">
+        <v>28881</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-19721</v>
+      </c>
+      <c r="N12" t="n">
+        <v>-3.96</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>主力積極賣出</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>4958</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>臻鼎-KY</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>178</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="E13" t="n">
+        <v>39138</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <v>-569</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4701</v>
+      </c>
+      <c r="H13" t="n">
+        <v>115</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-1119</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1465</v>
+      </c>
+      <c r="K13" t="n">
+        <v>31044</v>
+      </c>
+      <c r="L13" t="n">
+        <v>106786</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-267475</v>
+      </c>
+      <c r="N13" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>中性</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>6442</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>光聖</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1725</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>9.869999999999999</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5913</v>
+      </c>
+      <c r="F14" s="6" t="n">
+        <v>2005</v>
+      </c>
+      <c r="G14" t="n">
+        <v>491</v>
+      </c>
+      <c r="H14" t="n">
+        <v>153</v>
+      </c>
+      <c r="I14" t="n">
+        <v>297</v>
+      </c>
+      <c r="J14" t="n">
+        <v>264</v>
+      </c>
+      <c r="K14" t="n">
+        <v>4528</v>
+      </c>
+      <c r="L14" t="n">
+        <v>25675</v>
+      </c>
+      <c r="M14" t="n">
+        <v>-19146</v>
+      </c>
+      <c r="N14" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>偏多</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>3081</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>聯亞</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1095</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>9.609999999999999</v>
+      </c>
+      <c r="E15" t="n">
+        <v>903</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>1428</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-1126</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1432</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-290</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-678</v>
+      </c>
+      <c r="L15" t="n">
+        <v>-36</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>中性</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>3260</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>威剛</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>312.5</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>-5.59</v>
+      </c>
+      <c r="E16" t="n">
+        <v>23943</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <v>-1222</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-6703</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-282</v>
+      </c>
+      <c r="I16" t="n">
+        <v>965</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-243</v>
+      </c>
+      <c r="K16" t="n">
+        <v>280</v>
+      </c>
+      <c r="L16" t="n">
+        <v>4584</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>偏空</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>3265</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>台新科</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>136</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1285</v>
+      </c>
+      <c r="F17" s="7" t="n">
+        <v>-239</v>
+      </c>
+      <c r="G17" t="n">
+        <v>289</v>
+      </c>
+      <c r="H17" t="n">
+        <v>211</v>
+      </c>
+      <c r="I17" t="n">
+        <v>736</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-4</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-120</v>
+      </c>
+      <c r="L17" t="n">
+        <v>-784</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>主力積極買進</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>4979</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>華星光</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>314</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>-1.72</v>
+      </c>
+      <c r="E18" t="n">
+        <v>29576</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>2460</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-5142</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2508</v>
+      </c>
+      <c r="I18" t="n">
+        <v>2918</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-270</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-971</v>
+      </c>
+      <c r="L18" t="n">
+        <v>-2749</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>中性</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>